<commit_message>
Fix: Se arreglaron graficas
</commit_message>
<xml_diff>
--- a/AlgoritmosOrdenamiento/Excel_Datos_Algoritmos_Ordenamiento.xlsx
+++ b/AlgoritmosOrdenamiento/Excel_Datos_Algoritmos_Ordenamiento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elkyn\source\repos\AlgoritmosOrdenamiento\AlgoritmosOrdenamiento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD01AE5-9182-4411-A5DE-EBC38D7129DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98515003-02F0-463C-9068-9B86682B2F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{813B899E-915E-4DF5-83F4-AF032A48EDE5}"/>
   </bookViews>
@@ -261,13 +261,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -321,11 +321,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="es-MX"/>
-              <a:t>Tiempo</a:t>
+              <a:t>Arreglo</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="es-MX" baseline="0"/>
-              <a:t> de ejecucion Arreglos pequenos </a:t>
+              <a:t> Pequeño</a:t>
             </a:r>
             <a:endParaRPr lang="es-MX"/>
           </a:p>
@@ -335,8 +335,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.19225"/>
-          <c:y val="3.7037037037037035E-2"/>
+          <c:x val="0.41520695640951488"/>
+          <c:y val="5.1214660169029848E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -388,6 +388,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>('Algoritmos de Ordenamiento'!$A$5:$A$9,'Algoritmos de Ordenamiento'!$A$18:$A$22,'Algoritmos de Ordenamiento'!$A$27:$A$31,'Algoritmos de Ordenamiento'!$A$36:$A$40,'Algoritmos de Ordenamiento'!$A$45:$A$49,'Algoritmos de Ordenamiento'!$A$54:$A$58)</c:f>
@@ -592,8 +650,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -798,445 +857,6 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="es-MX"/>
-              <a:t>Arreglo</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="es-MX" baseline="0"/>
-              <a:t> Mediano</a:t>
-            </a:r>
-            <a:endParaRPr lang="es-MX"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>('Algoritmos de Ordenamiento'!$A$18:$A$22,'Algoritmos de Ordenamiento'!$A$27:$A$31,'Algoritmos de Ordenamiento'!$A$36:$A$40,'Algoritmos de Ordenamiento'!$A$45:$A$49,'Algoritmos de Ordenamiento'!$A$54:$A$58)</c:f>
-              <c:strCache>
-                <c:ptCount val="25"/>
-                <c:pt idx="0">
-                  <c:v>Selection Sort Intento 1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Selection Sort Intento 2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Selection Sort Intento 3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Selection Sort Intento 4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Selection Sort Intento 5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Insertion Sort Intento 1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Insertion Sort Intento 2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Insertion Sort Intento 3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Insertion Sort Intento 4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Insertion Sort Intento 5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Quick Sort Intento 1</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Quick Sort Intento 2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Quick Sort Intento 3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Quick Sort Intento 4</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Quick Sort Intento 5</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Merge sort Intento 1</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Merge sort Intento 2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Merge sort Intento 3</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Merge sort Intento 4</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Merge sort Intento 5</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>Heap Sort intento 1</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>Heap Sort intento 2</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Heap Sort intento 3</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>Heap Sort intento 4</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Heap Sort intento 5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>('Algoritmos de Ordenamiento'!$C$18:$C$22,'Algoritmos de Ordenamiento'!$C$27:$C$31,'Algoritmos de Ordenamiento'!$C$36:$C$40,'Algoritmos de Ordenamiento'!$C$45:$C$49,'Algoritmos de Ordenamiento'!$C$54:$C$58)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
-                <c:pt idx="0">
-                  <c:v>3059</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2959</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3033</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3033</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3113</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1867</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2070</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1984</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2012</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1947</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>16</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E657-4B19-8CC0-6092F077021E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="341661248"/>
-        <c:axId val="341664128"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="341661248"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="341664128"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="341664128"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="341661248"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="es-MX"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="es-MX"/>
               <a:t>Arreglo Grande</a:t>
             </a:r>
           </a:p>
@@ -1319,6 +939,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>('Algoritmos de Ordenamiento'!$A$5:$A$9,'Algoritmos de Ordenamiento'!$A$18:$A$22,'Algoritmos de Ordenamiento'!$A$27:$A$31,'Algoritmos de Ordenamiento'!$A$36:$A$40,'Algoritmos de Ordenamiento'!$A$45:$A$49,'Algoritmos de Ordenamiento'!$A$54:$A$58)</c:f>
@@ -1523,8 +1201,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -1639,6 +1318,520 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="227275856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-MX"/>
+              <a:t>Arreglo</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-MX" baseline="0"/>
+              <a:t> Mediano</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>('Algoritmos de Ordenamiento'!$A$5:$A$9,'Algoritmos de Ordenamiento'!$A$18:$A$22,'Algoritmos de Ordenamiento'!$A$27:$A$31,'Algoritmos de Ordenamiento'!$A$36:$A$40,'Algoritmos de Ordenamiento'!$A$45:$A$49,'Algoritmos de Ordenamiento'!$A$54:$A$58)</c:f>
+              <c:strCache>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>Bubble sort Intento 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble sort Intento 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Bubble sort Intento 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Bubble sort Intento 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Bubble sort Intento 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Selection Sort Intento 1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Selection Sort Intento 2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Selection Sort Intento 3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Selection Sort Intento 4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Selection Sort Intento 5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Insertion Sort Intento 1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Insertion Sort Intento 2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Insertion Sort Intento 3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Insertion Sort Intento 4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Insertion Sort Intento 5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Quick Sort Intento 1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Quick Sort Intento 2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Quick Sort Intento 3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Quick Sort Intento 4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Quick Sort Intento 5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Merge sort Intento 1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Merge sort Intento 2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Merge sort Intento 3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Merge sort Intento 4</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Merge sort Intento 5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Heap Sort intento 1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Heap Sort intento 2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Heap Sort intento 3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Heap Sort intento 4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Heap Sort intento 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Algoritmos de Ordenamiento'!$C$5:$C$9,'Algoritmos de Ordenamiento'!$C$18:$C$22,'Algoritmos de Ordenamiento'!$C$27:$C$31,'Algoritmos de Ordenamiento'!$C$36:$C$40,'Algoritmos de Ordenamiento'!$C$45:$C$49,'Algoritmos de Ordenamiento'!$C$54:$C$58)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>11160</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10917</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10938</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11213</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3059</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2959</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3033</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3033</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3113</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1867</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2070</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1984</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1947</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A19A-45F8-8C4F-5FB3AB8CB26A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="818201247"/>
+        <c:axId val="818202687"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="818201247"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="818202687"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="818202687"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="818201247"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3328,15 +3521,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>131618</xdr:colOff>
+      <xdr:colOff>135427</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>96982</xdr:rowOff>
+      <xdr:rowOff>93172</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>755072</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>149678</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>138546</xdr:rowOff>
+      <xdr:rowOff>134736</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3364,22 +3557,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>147918</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>53788</xdr:rowOff>
+      <xdr:colOff>45446</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>56062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>775448</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>107576</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>163285</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>25309</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Gráfico 4">
+        <xdr:cNvPr id="6" name="Gráfico 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5402605D-E41E-A615-72D9-3B953A8FDE94}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFEAE5C1-84F7-A013-6B48-04C46E550803}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3400,22 +3593,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>43542</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>59872</xdr:rowOff>
+      <xdr:colOff>142473</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>130292</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>642257</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>27214</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>176893</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>168344</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Gráfico 5">
+        <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFEAE5C1-84F7-A013-6B48-04C46E550803}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAF4A427-21E1-CD6C-CD72-AA2A5726F704}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3755,8 +3948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{334B73C9-72A8-438E-B98A-CBF01992EF36}">
   <dimension ref="A3:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10:G12"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3769,11 +3962,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
@@ -3805,7 +3998,7 @@
       <c r="D5" s="3">
         <v>43867</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="9" t="s">
         <v>4</v>
       </c>
       <c r="G5" s="2">
@@ -3825,7 +4018,7 @@
       <c r="D6" s="3">
         <v>44193</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="9" t="s">
         <v>3</v>
       </c>
       <c r="G6" s="2">
@@ -3890,25 +4083,25 @@
         <f>SUM(D5:D9)</f>
         <v>218945</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="10"/>
+      <c r="G10" s="11"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
@@ -4010,11 +4203,11 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
@@ -4115,11 +4308,11 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B35" s="1" t="s">
@@ -4220,11 +4413,11 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
       <c r="F43" s="7"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -4326,11 +4519,11 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B52" s="9" t="s">
+      <c r="B52" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B53" s="1" t="s">
@@ -4448,15 +4641,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010050099B6F8806D347B561049A506329A9" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bbf25b7e0c23f2f9b3c94f3fe642789f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d3f30225-3568-47fb-8891-4e13451e7e2a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="22568874a786bfa4a866f942648d7933" ns3:_="">
     <xsd:import namespace="d3f30225-3568-47fb-8891-4e13451e7e2a"/>
@@ -4646,6 +4830,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -4653,14 +4846,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2216D6A-323A-41C6-A4E3-6178E6695996}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58DE0C67-68A2-4CD8-9B7A-0DE8CC47D81D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4674,6 +4859,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2216D6A-323A-41C6-A4E3-6178E6695996}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>